<commit_message>
Registro en Excel Total CLP Versión Run en Edge
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test.xlsx
+++ b/src/test/resources/filepath/Test.xlsx
@@ -34,12 +34,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
   <si>
     <t>$ 27.307 CLP 14-10-20</t>
   </si>
   <si>
     <t>Prop Destacada 0,95 UF</t>
+  </si>
+  <si>
+    <t>$ 27.312 CLP 15-10-20</t>
+  </si>
+  <si>
+    <t>$ 27.318 CLP 16-10-20</t>
   </si>
 </sst>
 </file>
@@ -392,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A62913-EEAF-4FB6-B95A-B8F46E178A92}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -424,6 +430,66 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>